<commit_message>
Change Requirements/Code Phases Defects & Clean up ignored files
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\An3\VVS\proiect_vss_DoubleD\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMI\Anul III\Semestrul II\Verificarea si validarea sistemelor soft\proiect_vss_DoubleD\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB8249E-B041-414A-9CCB-555AA9CD133A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B9786D-FCBE-4E87-B664-F7A504EB6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -19,11 +19,22 @@
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -127,33 +138,12 @@
     <t>R02</t>
   </si>
   <si>
-    <t>R06</t>
-  </si>
-  <si>
-    <t>Primul paragraf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nu se cunosc exact actiunile pe care le face un user. Desi se mentioneaza ca "aplicatia gestioneaza" doua tipuri de obiecte, ceea ce duce cu gandul la operatii CRUD, ar trebui dezvoltat la ceea ce se refera userul si ce isi doreste el sa faca aplicatia cand se refera la "gestionare". </t>
-  </si>
-  <si>
-    <t>Prima pagina</t>
-  </si>
-  <si>
     <t>F01</t>
   </si>
   <si>
-    <t xml:space="preserve">F01 mentioneaza adaugarea obiectelor cu anumite detalii, insa niciunul dintre acestea nu apar in cerinta. Se specifica faptul ca informatiile sunt preluate dintr-un fisier text, insa ar trebui detaliat continutul acelui fisier. In plus, ar trebui specificat daca detaliile ambelor entitati sunt preluate din acelasi fisier sau din fisiere diferite. </t>
-  </si>
-  <si>
-    <t>Din cauza lipsei de detalii din specificatie, nu putem afirma cu siguranta daca exista cerinte care lipsesc sau nu. Totusi, sunt sanse ca acestea sa nu acopere intru totul ceea ce s-a dorit de la aplicatie.</t>
-  </si>
-  <si>
     <t>F02</t>
   </si>
   <si>
-    <t>Cautarea doar dupa nume este destul de restrictiva, poate ar trebui sa se permita cautarea si dupa alte campuri ale obiectelor (de exemplu, producatorul unei piese).</t>
-  </si>
-  <si>
     <t>Ateodoresi Denisa</t>
   </si>
   <si>
@@ -163,46 +153,25 @@
     <t>30min</t>
   </si>
   <si>
-    <t>C08</t>
-  </si>
-  <si>
     <t>InventoryRepository.java, liniile 37, 39, 90, 92, 158</t>
   </si>
   <si>
     <t>C01</t>
   </si>
   <si>
-    <t>In cazul in care se incearca deschiderea unui fisier, iar acesta nu exista, se intra in block-ul de catch unde nu sunt procesate mesaje de eroare personalizate, ci doar se afiseaza eroarea complexa returnata de exceptie.</t>
-  </si>
-  <si>
     <t>F04</t>
   </si>
   <si>
-    <t>F04 mentioneaza stergerea unui produs sau a unei piese, insa cerinta ar trebui sa ofere explicatii si pentru ceea ce se intampla atunci cand se incearca stergerea unei piese care este folosita la unul sau la mai multe produse.</t>
-  </si>
-  <si>
     <t>C07</t>
   </si>
   <si>
     <t>AddPartController.java, 171, AddProductController.java, 219, ModifyPartController.java, 204, ModifyProductController.java, 214</t>
   </si>
   <si>
-    <t>Product.java, linia 99, Inventory.java, liniile 47, 101</t>
-  </si>
-  <si>
     <t>30 min</t>
   </si>
   <si>
     <t>In momentul verificarii input ului primit din UI, se arunca NumberFormatException in cazul in care campurile care trebuie transformate in numere sunt goale sau sunt completate cu valori care nu reprezinta numere. In acest caz, user ul primeste ca si output un mesaj care ii spune ca unele campuri sunt goale, insa acest lucru este incorect, iar mesajul afisat ar trebui sa surprinda concret cauza problemei. In plus, alertul ar trebui sa fie de tip ERROR, nu INFORMATION.</t>
-  </si>
-  <si>
-    <t>Cele trei instructiuni conditionale nu respecta partea de cautare din cerinta, intrucat cautarea ar trebui facuta dupa nume sau producator, dar codul incearca sa faca acea cautare si dupa ID (in cazul in care nu se gaseste nimic dupa nume).</t>
-  </si>
-  <si>
-    <t>Inventory.java, liniile 50-53</t>
-  </si>
-  <si>
-    <t>Liniile respective se afla in interiorul metodei ce returneaza produsul gasit pe baza unui string dat de utilizator. Daca nu gaseste niciun produs, creeaza un produs cu valori nule/0 si il returneaza, ceea ce este complet incorect --&gt; metoda trebuie sa returneze null in acest caz.</t>
   </si>
   <si>
     <t>A01</t>
@@ -419,6 +388,72 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):30 min</t>
+  </si>
+  <si>
+    <t>Nu se specifica tipul aplicatiei cerute (web, desktop, mobilă, etc).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desi se mentioneaza ca "aplicatia gestioneaza" doua tipuri de obiecte, ceea ce duce cu gandul la operatii CRUD, nu se mentioneaza exact ce actiuni sa permita aplicatia in acest sens. </t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>Nu se specifica rezultatul cautarii (cum se afiseaza elementele obtinute).</t>
+  </si>
+  <si>
+    <t>F04 mentioneaza stergerea unui produs sau a unei piese, insa cerinta ar trebui sa ofere explicatii si pentru ceea ce se intampla atunci cand se incearca stergerea unei piese care este folosita la unul sau la mai multe produse (daca este sau nu un impediment).</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
+    <t>Nu se specifica informatiile pe care le poate actualiza userul.</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Nu se mentioneaza comportamentul aplicatiei la pornire/initializare.</t>
+  </si>
+  <si>
+    <t>Cerintele nu surprind interactiunea dintre utilizator si interfata aplicatiei</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>F01 mentioneaza adaugarea obiectelor cu anumite detalii, insa nu se specifica daca si fisierul text contine acele informatii si sub ce forma.</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>Product.java, Part.java</t>
+  </si>
+  <si>
+    <t>Logica pentru validarea unei entitati ar trebui sa se afle intr-o clasa separata (un validator, de exemplu) si nu in interiorul entitatii respective.</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>In cazul in care se incearca deschiderea unui fisier, iar acesta nu exista, se intra in block-ul de catch unde nu sunt procesate mesaje de eroare personalizate, ci doar se afiseaza eroarea complexa returnata de exceptie in terminal.</t>
+  </si>
+  <si>
+    <t>La citirea din fisier nu se verifica daca valorile sunt de tipul cerut; de exemplu, daca se asteapta o valoare de tip int, nu se verifica daca acea valoare citita din fisier este int sau string; aplicatia se comporta ca si cum ar fi int.</t>
+  </si>
+  <si>
+    <t>InventoryRepository.java, liniile 43, 96</t>
+  </si>
+  <si>
+    <t>Inventory.java, liniile 44, 99</t>
+  </si>
+  <si>
+    <t>Cautarea ar trebui facuta dupa nume, insa codul returneaza un produs/o piesa si in cazul in care nu exista o potrivire cu numele, dar exista cu ID-ul.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +561,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,8 +586,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -621,11 +698,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,51 +771,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -715,6 +784,87 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,8 +1209,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1218,7 @@
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="68.33203125" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
     <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
@@ -1080,19 +1230,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1106,7 +1256,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1116,15 +1266,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="45"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1134,10 +1284,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="47"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1149,17 +1299,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
-        <v>44989</v>
-      </c>
-      <c r="E7" s="24"/>
+      <c r="D7" s="41">
+        <v>44995</v>
+      </c>
+      <c r="E7" s="42"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1175,106 +1325,116 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="E11" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E14" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="40"/>
+      <c r="D15" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="39"/>
+      <c r="D16" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -1354,11 +1514,13 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:E2"/>
@@ -1378,7 +1540,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -1398,19 +1560,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1424,7 +1586,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1434,15 +1596,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="48"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1452,10 +1614,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="50"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1467,15 +1629,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
@@ -1496,11 +1658,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1509,11 +1671,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1522,11 +1684,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1535,11 +1697,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1547,12 +1709,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>67</v>
+      <c r="C14" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="40" t="s">
-        <v>89</v>
+      <c r="E14" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1664,19 +1826,19 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="41"/>
-      <c r="C28" s="42" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="43"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1700,8 +1862,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1710,7 +1872,7 @@
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="58.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="64" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
@@ -1721,19 +1883,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1747,7 +1909,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1757,15 +1919,15 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="51"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1775,10 +1937,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="53"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1790,17 +1952,17 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
-        <v>44990</v>
-      </c>
-      <c r="E7" s="24"/>
+      <c r="D7" s="41">
+        <v>44995</v>
+      </c>
+      <c r="E7" s="42"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1816,73 +1978,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="C12" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="39"/>
+      <c r="D13" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
@@ -2034,11 +2200,12 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="D4:E4"/>
@@ -2058,7 +2225,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2080,19 +2247,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2105,8 +2272,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="39" t="s">
-        <v>43</v>
+      <c r="I3" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -2116,13 +2283,13 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="38" t="s">
-        <v>44</v>
+      <c r="I4" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -2132,8 +2299,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2145,8 +2312,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2171,16 +2338,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2189,16 +2356,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2207,16 +2374,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
@@ -2225,16 +2392,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -2243,16 +2410,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2416,11 +2583,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="C32" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added observer remark. Changed C08 errors to C04
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMI\Anul III\Semestrul II\Verificarea si validarea sistemelor soft\proiect_vss_DoubleD\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\An3\VVS\proiect_vss_DoubleD\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B9786D-FCBE-4E87-B664-F7A504EB6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A24C6B-CE5C-4B57-A5E8-ED5E4F10C421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40380" yWindow="0" windowWidth="17220" windowHeight="15600" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -19,17 +19,6 @@
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -196,9 +185,6 @@
   </si>
   <si>
     <t>A07</t>
-  </si>
-  <si>
-    <t>Da. Poate fi identificat pattern-ul MVC. Exista separare clara a claselor in cele 3 parti ale pattern-ului Model/View/Controller</t>
   </si>
   <si>
     <t>Use isEmpty() to check wheteher the collection is empty or not</t>
@@ -455,18 +441,29 @@
   <si>
     <t>Cautarea ar trebui facuta dupa nume, insa codul returneaza un produs/o piesa si in cazul in care nu exista o potrivire cu numele, dar exista cu ID-ul.</t>
   </si>
+  <si>
+    <t>Da. Poate fi identificat pattern-ul MVC. Exista separare clara a claselor in cele 3 parti ale pattern-ului Model/View/Controller.
+Si pattern-ul Observer, pe liste.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -739,132 +736,135 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,8 +1209,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,10 +1333,10 @@
         <v>32</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1361,10 +1361,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1373,13 +1373,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1392,7 +1392,7 @@
         <v>41</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1402,10 +1402,10 @@
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="36" t="s">
         <v>82</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1415,10 +1415,10 @@
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1427,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="32" t="s">
         <v>85</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1540,8 +1540,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="B10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1691,7 +1691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1713,8 +1713,8 @@
         <v>53</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="25" t="s">
-        <v>75</v>
+      <c r="E14" s="56" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1862,8 +1862,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1983,13 +1983,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2016,10 +2016,10 @@
         <v>40</v>
       </c>
       <c r="D12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2029,10 +2029,10 @@
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>97</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -2041,13 +2041,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2225,8 +2225,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2338,16 +2338,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2356,16 +2356,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2374,16 +2374,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
@@ -2392,16 +2392,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -2410,16 +2410,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2584,7 +2584,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="55"/>
       <c r="E32" s="55"/>

</xml_diff>